<commit_message>
Avances 25 noviembre 2017
</commit_message>
<xml_diff>
--- a/articulo_dfa/info_tecnico.xlsx
+++ b/articulo_dfa/info_tecnico.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="parche_EpocasMOR" sheetId="5" r:id="rId3"/>
     <sheet name="Epocas_todas" sheetId="3" r:id="rId4"/>
     <sheet name="Heuristico" sheetId="4" r:id="rId5"/>
+    <sheet name="General_old" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="68">
   <si>
     <t>Nombre_archivo</t>
   </si>
@@ -1476,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="N2" s="5">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O2" s="5">
         <v>0</v>
@@ -1606,7 +1607,7 @@
         <v>2</v>
       </c>
       <c r="Q2" s="5">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="R2" s="5">
         <v>0</v>
@@ -1765,16 +1766,16 @@
         <v>3</v>
       </c>
       <c r="N5" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="O5" s="1">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P5" s="1">
         <v>3</v>
       </c>
       <c r="Q5" s="1">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="R5" s="1">
         <v>0</v>
@@ -1821,19 +1822,19 @@
         <v>2</v>
       </c>
       <c r="N6" s="5">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="O6" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P6" s="5">
         <v>2</v>
       </c>
       <c r="Q6" s="5">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="R6" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1989,16 +1990,16 @@
         <v>1</v>
       </c>
       <c r="N9" s="4">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O9" s="4">
         <v>30</v>
       </c>
       <c r="P9" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="4">
         <v>1</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>58</v>
       </c>
       <c r="R9" s="4">
         <v>30</v>
@@ -2857,8 +2858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4239,8 +4240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N270"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H2:H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9997,7 +9998,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:N15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10074,20 +10077,19 @@
         <v>10</v>
       </c>
       <c r="D2" s="143">
-        <f>EpocasMOR!A11</f>
-        <v>721</v>
+        <v>980</v>
       </c>
       <c r="E2" s="143">
         <f>EpocasMOR!A2</f>
         <v>712</v>
       </c>
       <c r="F2" s="5">
-        <f>E2-10</f>
-        <v>702</v>
+        <f>E2-10*(30/C2)</f>
+        <v>682</v>
       </c>
       <c r="G2" s="5">
         <f>(F2-1)*C2</f>
-        <v>7010</v>
+        <v>6810</v>
       </c>
       <c r="H2" s="5">
         <f>INT(G2/(60*60))</f>
@@ -10095,15 +10097,15 @@
       </c>
       <c r="I2" s="5">
         <f>INT((G2-60*60*H2)/60)</f>
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J2" s="5">
         <f>G2-60*60*H2-60*I2</f>
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="K2" s="5">
         <f>D2*C2</f>
-        <v>7210</v>
+        <v>9800</v>
       </c>
       <c r="L2" s="5">
         <f>INT(K2/(60*60))</f>
@@ -10111,11 +10113,11 @@
       </c>
       <c r="M2" s="5">
         <f>INT((K2-60*60*L2)/60)</f>
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N2" s="5">
         <f>K2-60*60*L2-60*M2</f>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -10131,7 +10133,6 @@
         <v>30</v>
       </c>
       <c r="D3" s="145">
-        <f>EpocasMOR!B11</f>
         <v>192</v>
       </c>
       <c r="E3" s="145">
@@ -10139,7 +10140,7 @@
         <v>183</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F15" si="0">E3-10</f>
+        <f t="shared" ref="F3:F15" si="0">E3-10*(30/C3)</f>
         <v>173</v>
       </c>
       <c r="G3" s="1">
@@ -10188,7 +10189,6 @@
         <v>30</v>
       </c>
       <c r="D4" s="143">
-        <f>EpocasMOR!C11</f>
         <v>140</v>
       </c>
       <c r="E4" s="143">
@@ -10245,8 +10245,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="145">
-        <f>EpocasMOR!D11</f>
-        <v>1195</v>
+        <v>1244</v>
       </c>
       <c r="E5" s="145">
         <f>EpocasMOR!D2</f>
@@ -10254,11 +10253,11 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>1174</v>
+        <v>1154</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>11730</v>
+        <v>11530</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="2"/>
@@ -10266,15 +10265,15 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="5"/>
-        <v>11950</v>
+        <v>12440</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="6"/>
@@ -10282,11 +10281,11 @@
       </c>
       <c r="M5" s="1">
         <f t="shared" si="7"/>
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -10302,8 +10301,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="143">
-        <f>EpocasMOR!E11</f>
-        <v>833</v>
+        <v>853</v>
       </c>
       <c r="E6" s="143">
         <f>EpocasMOR!E2</f>
@@ -10311,11 +10309,11 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>814</v>
+        <v>794</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="1"/>
-        <v>8130</v>
+        <v>7930</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="2"/>
@@ -10323,15 +10321,15 @@
       </c>
       <c r="I6" s="5">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="5"/>
-        <v>8330</v>
+        <v>8530</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="6"/>
@@ -10339,11 +10337,11 @@
       </c>
       <c r="M6" s="5">
         <f t="shared" si="7"/>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="N6" s="5">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -10359,7 +10357,6 @@
         <v>30</v>
       </c>
       <c r="D7" s="146">
-        <f>EpocasMOR!F11</f>
         <v>176</v>
       </c>
       <c r="E7" s="146">
@@ -10416,7 +10413,6 @@
         <v>30</v>
       </c>
       <c r="D8" s="147">
-        <f>EpocasMOR!G11</f>
         <v>251</v>
       </c>
       <c r="E8" s="147">
@@ -10473,8 +10469,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="146">
-        <f>EpocasMOR!H11</f>
-        <v>706</v>
+        <v>726</v>
       </c>
       <c r="E9" s="146">
         <f>EpocasMOR!H2</f>
@@ -10482,11 +10477,11 @@
       </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
-        <v>687</v>
+        <v>667</v>
       </c>
       <c r="G9" s="4">
         <f t="shared" si="1"/>
-        <v>6860</v>
+        <v>6660</v>
       </c>
       <c r="H9" s="4">
         <f t="shared" si="2"/>
@@ -10494,27 +10489,27 @@
       </c>
       <c r="I9" s="4">
         <f t="shared" si="3"/>
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K9" s="4">
         <f t="shared" si="5"/>
-        <v>7060</v>
+        <v>7260</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M9" s="4">
         <f t="shared" si="7"/>
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="N9" s="4">
         <f t="shared" si="8"/>
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -10530,7 +10525,6 @@
         <v>30</v>
       </c>
       <c r="D10" s="147">
-        <f>EpocasMOR!I11</f>
         <v>378</v>
       </c>
       <c r="E10" s="147">
@@ -10587,7 +10581,6 @@
         <v>30</v>
       </c>
       <c r="D11" s="146">
-        <f>EpocasMOR!J11</f>
         <v>610</v>
       </c>
       <c r="E11" s="146">
@@ -10644,7 +10637,6 @@
         <v>30</v>
       </c>
       <c r="D12" s="148">
-        <f>EpocasMOR!K11</f>
         <v>289</v>
       </c>
       <c r="E12" s="148">
@@ -10701,7 +10693,6 @@
         <v>30</v>
       </c>
       <c r="D13" s="149">
-        <f>EpocasMOR!L11</f>
         <v>410</v>
       </c>
       <c r="E13" s="149">
@@ -10758,7 +10749,6 @@
         <v>30</v>
       </c>
       <c r="D14" s="148">
-        <f>EpocasMOR!M11</f>
         <v>220</v>
       </c>
       <c r="E14" s="148">
@@ -10815,7 +10805,6 @@
         <v>30</v>
       </c>
       <c r="D15" s="149">
-        <f>EpocasMOR!N11</f>
         <v>148</v>
       </c>
       <c r="E15" s="149">
@@ -10857,6 +10846,879 @@
       <c r="N15" s="6">
         <f t="shared" si="8"/>
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="150" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="150" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="7">
+        <v>59</v>
+      </c>
+      <c r="E2" s="151">
+        <v>107</v>
+      </c>
+      <c r="F2" s="151">
+        <v>29</v>
+      </c>
+      <c r="G2" s="7">
+        <v>12</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="160">
+        <v>200</v>
+      </c>
+      <c r="L2" s="7">
+        <v>10</v>
+      </c>
+      <c r="M2" s="5">
+        <v>1</v>
+      </c>
+      <c r="N2" s="5">
+        <v>56</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>1</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="8">
+        <v>72</v>
+      </c>
+      <c r="E3" s="152">
+        <v>113</v>
+      </c>
+      <c r="F3" s="152">
+        <v>30</v>
+      </c>
+      <c r="G3" s="8">
+        <v>9</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="8">
+        <v>512</v>
+      </c>
+      <c r="L3" s="8">
+        <v>30</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>25</v>
+      </c>
+      <c r="O3" s="1">
+        <v>30</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>36</v>
+      </c>
+      <c r="R3" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="7">
+        <v>78</v>
+      </c>
+      <c r="E4" s="151">
+        <v>102</v>
+      </c>
+      <c r="F4" s="151">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7">
+        <v>5</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="7">
+        <v>512</v>
+      </c>
+      <c r="L4" s="7">
+        <v>30</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>48</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>10</v>
+      </c>
+      <c r="R4" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="8">
+        <v>65</v>
+      </c>
+      <c r="E5" s="152">
+        <v>107.5</v>
+      </c>
+      <c r="F5" s="152">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8">
+        <v>9</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="160">
+        <v>200</v>
+      </c>
+      <c r="L5" s="8">
+        <v>10</v>
+      </c>
+      <c r="M5" s="1">
+        <v>3</v>
+      </c>
+      <c r="N5" s="1">
+        <v>15</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>20</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>26</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="7">
+        <v>67</v>
+      </c>
+      <c r="E6" s="151">
+        <v>115</v>
+      </c>
+      <c r="F6" s="151">
+        <v>30</v>
+      </c>
+      <c r="G6" s="7">
+        <v>11</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="160">
+        <v>200</v>
+      </c>
+      <c r="L6" s="7">
+        <v>10</v>
+      </c>
+      <c r="M6" s="5">
+        <v>2</v>
+      </c>
+      <c r="N6" s="5">
+        <v>15</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>19</v>
+      </c>
+      <c r="R6" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="9">
+        <v>68</v>
+      </c>
+      <c r="E7" s="153">
+        <v>81</v>
+      </c>
+      <c r="F7" s="154">
+        <v>28</v>
+      </c>
+      <c r="G7" s="9">
+        <v>5</v>
+      </c>
+      <c r="H7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="9">
+        <v>512</v>
+      </c>
+      <c r="L7" s="9">
+        <v>30</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4">
+        <v>17</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>28</v>
+      </c>
+      <c r="R7" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="10">
+        <v>63</v>
+      </c>
+      <c r="E8" s="155">
+        <v>90</v>
+      </c>
+      <c r="F8" s="155">
+        <v>29</v>
+      </c>
+      <c r="G8" s="10">
+        <v>9</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="10">
+        <v>512</v>
+      </c>
+      <c r="L8" s="10">
+        <v>30</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3">
+        <v>55</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>6</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="9">
+        <v>69</v>
+      </c>
+      <c r="E9" s="153">
+        <v>85</v>
+      </c>
+      <c r="F9" s="153">
+        <v>26</v>
+      </c>
+      <c r="G9" s="9">
+        <v>9</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="160">
+        <v>200</v>
+      </c>
+      <c r="L9" s="9">
+        <v>10</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <v>53</v>
+      </c>
+      <c r="O9" s="4">
+        <v>30</v>
+      </c>
+      <c r="P9" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>58</v>
+      </c>
+      <c r="R9" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="10">
+        <v>65</v>
+      </c>
+      <c r="E10" s="155">
+        <v>87</v>
+      </c>
+      <c r="F10" s="155">
+        <v>25</v>
+      </c>
+      <c r="G10" s="10">
+        <v>11</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="10">
+        <v>512</v>
+      </c>
+      <c r="L10" s="10">
+        <v>30</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2</v>
+      </c>
+      <c r="N10" s="3">
+        <v>58</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>9</v>
+      </c>
+      <c r="R10" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>83</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="9">
+        <v>73</v>
+      </c>
+      <c r="E11" s="153">
+        <v>96</v>
+      </c>
+      <c r="F11" s="153">
+        <v>29</v>
+      </c>
+      <c r="G11" s="9">
+        <v>8</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="9">
+        <v>512</v>
+      </c>
+      <c r="L11" s="9">
+        <v>30</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>50</v>
+      </c>
+      <c r="O11" s="4">
+        <v>30</v>
+      </c>
+      <c r="P11" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>5</v>
+      </c>
+      <c r="R11" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="12">
+        <v>71</v>
+      </c>
+      <c r="E12" s="156">
+        <v>83.5</v>
+      </c>
+      <c r="F12" s="157">
+        <v>21</v>
+      </c>
+      <c r="G12" s="12">
+        <v>9</v>
+      </c>
+      <c r="H12" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="12">
+        <v>512</v>
+      </c>
+      <c r="L12" s="12">
+        <v>30</v>
+      </c>
+      <c r="M12" s="2">
+        <v>2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>12</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>25</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="11">
+        <v>61</v>
+      </c>
+      <c r="E13" s="158">
+        <v>114</v>
+      </c>
+      <c r="F13" s="158">
+        <v>28</v>
+      </c>
+      <c r="G13" s="11">
+        <v>9</v>
+      </c>
+      <c r="H13" s="11">
+        <v>-1</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="11">
+        <v>512</v>
+      </c>
+      <c r="L13" s="11">
+        <v>30</v>
+      </c>
+      <c r="M13" s="6">
+        <v>1</v>
+      </c>
+      <c r="N13" s="6">
+        <v>53</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0</v>
+      </c>
+      <c r="P13" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>25</v>
+      </c>
+      <c r="R13" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="12">
+        <v>50</v>
+      </c>
+      <c r="E14" s="156">
+        <v>117</v>
+      </c>
+      <c r="F14" s="156">
+        <v>30</v>
+      </c>
+      <c r="G14" s="12">
+        <v>22</v>
+      </c>
+      <c r="H14" s="12">
+        <v>-1</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="12">
+        <v>512</v>
+      </c>
+      <c r="L14" s="12">
+        <v>30</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2">
+        <v>35</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>50</v>
+      </c>
+      <c r="R14" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>99</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="14">
+        <v>71</v>
+      </c>
+      <c r="E15" s="159">
+        <v>111</v>
+      </c>
+      <c r="F15" s="159">
+        <v>28</v>
+      </c>
+      <c r="G15" s="14">
+        <v>9</v>
+      </c>
+      <c r="H15" s="14">
+        <v>-1</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="14">
+        <v>512</v>
+      </c>
+      <c r="L15" s="14">
+        <v>30</v>
+      </c>
+      <c r="M15" s="13">
+        <v>1</v>
+      </c>
+      <c r="N15" s="13">
+        <v>3</v>
+      </c>
+      <c r="O15" s="13">
+        <v>30</v>
+      </c>
+      <c r="P15" s="13">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="13">
+        <v>14</v>
+      </c>
+      <c r="R15" s="13">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>